<commit_message>
fixing 21 yal final 5 apr home
</commit_message>
<xml_diff>
--- a/LOGS/20b5ede5-d85a-4dd1-a489-8eeefb513242/main_page_service_output/notes_standard_cropped_df.xlsx
+++ b/LOGS/20b5ede5-d85a-4dd1-a489-8eeefb513242/main_page_service_output/notes_standard_cropped_df.xlsx
@@ -659,6 +659,9 @@
       <c r="D2">
         <v>2021</v>
       </c>
+      <c r="E2">
+        <v>2021</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -673,6 +676,9 @@
       <c r="D3">
         <v>2021</v>
       </c>
+      <c r="E3">
+        <v>2021</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -687,6 +693,9 @@
       <c r="D4">
         <v>2021</v>
       </c>
+      <c r="E4">
+        <v>2021</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -701,6 +710,9 @@
       <c r="D5">
         <v>2021</v>
       </c>
+      <c r="E5">
+        <v>2021</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" t="s">
@@ -712,6 +724,9 @@
       <c r="D6">
         <v>2021</v>
       </c>
+      <c r="E6">
+        <v>2021</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
@@ -726,6 +741,9 @@
       <c r="D7">
         <v>2020</v>
       </c>
+      <c r="E7">
+        <v>2020</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
@@ -740,6 +758,9 @@
       <c r="D8">
         <v>2020</v>
       </c>
+      <c r="E8">
+        <v>2020</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
@@ -754,6 +775,9 @@
       <c r="D9">
         <v>2020</v>
       </c>
+      <c r="E9">
+        <v>2020</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
@@ -768,6 +792,9 @@
       <c r="D10">
         <v>2020</v>
       </c>
+      <c r="E10">
+        <v>2020</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" t="s">
@@ -777,6 +804,9 @@
         <v>18170313</v>
       </c>
       <c r="D11">
+        <v>2020</v>
+      </c>
+      <c r="E11">
         <v>2020</v>
       </c>
     </row>
@@ -820,6 +850,9 @@
       <c r="D2" t="s">
         <v>19</v>
       </c>
+      <c r="E2">
+        <v>2021</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -830,6 +863,9 @@
       </c>
       <c r="D3" t="s">
         <v>20</v>
+      </c>
+      <c r="E3">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -1495,6 +1531,9 @@
       <c r="D2">
         <v>2021</v>
       </c>
+      <c r="E2">
+        <v>2021</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -1509,6 +1548,9 @@
       <c r="D3">
         <v>2021</v>
       </c>
+      <c r="E3">
+        <v>2021</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -1523,6 +1565,9 @@
       <c r="D4">
         <v>2021</v>
       </c>
+      <c r="E4">
+        <v>2021</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -1537,6 +1582,9 @@
       <c r="D5">
         <v>2021</v>
       </c>
+      <c r="E5">
+        <v>2021</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -1551,6 +1599,9 @@
       <c r="D6">
         <v>2021</v>
       </c>
+      <c r="E6">
+        <v>2021</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
@@ -1565,6 +1616,9 @@
       <c r="D7">
         <v>2021</v>
       </c>
+      <c r="E7">
+        <v>2021</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
@@ -1579,6 +1633,9 @@
       <c r="D8">
         <v>2021</v>
       </c>
+      <c r="E8">
+        <v>2021</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
@@ -1593,6 +1650,9 @@
       <c r="D9">
         <v>2021</v>
       </c>
+      <c r="E9">
+        <v>2021</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
@@ -1607,6 +1667,9 @@
       <c r="D10">
         <v>2020</v>
       </c>
+      <c r="E10">
+        <v>2020</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -1621,6 +1684,9 @@
       <c r="D11">
         <v>2020</v>
       </c>
+      <c r="E11">
+        <v>2020</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
@@ -1635,6 +1701,9 @@
       <c r="D12">
         <v>2020</v>
       </c>
+      <c r="E12">
+        <v>2020</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
@@ -1649,6 +1718,9 @@
       <c r="D13">
         <v>2020</v>
       </c>
+      <c r="E13">
+        <v>2020</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
@@ -1663,6 +1735,9 @@
       <c r="D14">
         <v>2020</v>
       </c>
+      <c r="E14">
+        <v>2020</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
@@ -1677,6 +1752,9 @@
       <c r="D15">
         <v>2020</v>
       </c>
+      <c r="E15">
+        <v>2020</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
@@ -1691,8 +1769,11 @@
       <c r="D16">
         <v>2020</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -1703,6 +1784,9 @@
         <v>144455407</v>
       </c>
       <c r="D17">
+        <v>2020</v>
+      </c>
+      <c r="E17">
         <v>2020</v>
       </c>
     </row>
@@ -1746,6 +1830,9 @@
       <c r="D2" t="s">
         <v>19</v>
       </c>
+      <c r="E2">
+        <v>2021</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -1757,6 +1844,9 @@
       <c r="D3" t="s">
         <v>19</v>
       </c>
+      <c r="E3">
+        <v>2021</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -1768,6 +1858,9 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
+      <c r="E4">
+        <v>2021</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -1779,6 +1872,9 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
+      <c r="E5">
+        <v>2021</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -1790,6 +1886,9 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
+      <c r="E6">
+        <v>2021</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
@@ -1801,6 +1900,9 @@
       <c r="D7" t="s">
         <v>20</v>
       </c>
+      <c r="E7">
+        <v>2020</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
@@ -1812,6 +1914,9 @@
       <c r="D8" t="s">
         <v>20</v>
       </c>
+      <c r="E8">
+        <v>2020</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
@@ -1823,6 +1928,9 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
+      <c r="E9">
+        <v>2020</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
@@ -1834,6 +1942,9 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
+      <c r="E10">
+        <v>2020</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -1844,6 +1955,9 @@
       </c>
       <c r="D11" t="s">
         <v>20</v>
+      </c>
+      <c r="E11">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -1886,6 +2000,9 @@
       <c r="D2">
         <v>2021</v>
       </c>
+      <c r="E2">
+        <v>2021</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -1895,6 +2012,9 @@
         <v>33141783</v>
       </c>
       <c r="D3">
+        <v>2020</v>
+      </c>
+      <c r="E3">
         <v>2020</v>
       </c>
     </row>

</xml_diff>